<commit_message>
changed the names of all the assets to align with our naming convention
</commit_message>
<xml_diff>
--- a/Group1/asset_list.xlsx
+++ b/Group1/asset_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakri\Downloads\UNIVERSITY\2nd Year Game DEV\Maya Projects 2025-2026\Maya Assessment Group work\GamesProduction_Assessment3\Group1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronni\OneDrive\Documents\GitHub\GamesProduction_Assessment3\Group1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F740D5-984E-4FC0-AA90-A92F56E181CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554F98EC-574E-404A-96A5-164098A3CEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{3CADAA71-2A7C-4007-B115-84B73D999E61}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{3CADAA71-2A7C-4007-B115-84B73D999E61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="72">
   <si>
     <t>Number</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Monitor</t>
   </si>
   <si>
-    <t>Bedside Table</t>
-  </si>
-  <si>
     <t>Lamp</t>
   </si>
   <si>
@@ -205,6 +202,54 @@
   </si>
   <si>
     <t>Character 3 Head</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>Bulb</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>Blush</t>
+  </si>
+  <si>
+    <t>Makeup Tubes</t>
+  </si>
+  <si>
+    <t>Moomin Toy</t>
+  </si>
+  <si>
+    <t>Pen Holder</t>
+  </si>
+  <si>
+    <t>Photo Frame</t>
+  </si>
+  <si>
+    <t>Poster</t>
+  </si>
+  <si>
+    <t>Side Desk</t>
+  </si>
+  <si>
+    <t>Wardrobe</t>
   </si>
 </sst>
 </file>
@@ -572,17 +617,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2F9C19-B13F-4412-8794-4506A44CE5A9}">
   <dimension ref="A1:G300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="103" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="27.73046875" customWidth="1"/>
-    <col min="4" max="4" width="8.86328125" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -603,9 +648,9 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -617,9 +662,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -631,9 +676,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -645,7 +690,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -659,7 +704,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -670,7 +715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -681,7 +726,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -692,7 +737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -703,7 +748,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -723,7 +768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -731,10 +776,10 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -742,1568 +787,1613 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
         <v>51</v>
       </c>
-      <c r="D27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B33" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B34" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B35" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B36" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B37" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B40" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B129" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B133" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B134" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B144" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B145" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B146" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B147" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B148" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B149" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B151" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B152" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B153" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B154" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B155" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B156" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B157" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B158" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B159" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B160" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B161" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B162" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B163" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B164" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B165" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B166" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B167" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B168" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B169" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B170" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B171" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B172" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B173" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B174" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B175" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B176" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B177" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B178" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B179" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B180" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B181" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B182" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B183" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B184" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B185" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B186" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B187" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B188" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B189" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B190" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B191" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B192" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B193" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B194" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B195" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B196" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B197" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B198" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B199" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B200" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B201" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B202" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B203" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B204" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B205" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B206" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B207" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B208" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B209" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B210" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B211" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B212" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B213" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B214" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B215" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B216" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B217" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B218" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B219" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B220" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B221" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B222" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B223" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B224" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B225" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B226" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B227" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B228" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B229" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B230" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B231" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B232" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B233" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B234" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B235" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B236" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B237" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B238" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B239" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B240" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B241" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B242" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B243" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B244" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B245" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B246" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B247" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B248" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B249" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B250" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B251" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B252" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B253" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B254" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B255" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B256" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B257" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B258" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B259" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B260" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B261" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B262" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B263" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B264" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B265" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B266" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B267" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B268" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B269" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B270" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B271" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B272" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B273" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B274" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B275" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B276" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B277" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B278" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B279" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B280" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B281" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B282" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B283" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B284" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B285" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B286" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B287" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B288" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="289" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B289" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="290" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B290" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="291" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B291" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="292" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B292" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B293" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B294" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="295" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B295" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="296" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B296" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="297" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B297" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="298" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B298" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B299" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="300" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B300" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
trimsheets edited for bookshelf
</commit_message>
<xml_diff>
--- a/Group1/asset_list.xlsx
+++ b/Group1/asset_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakri\Downloads\UNIVERSITY\2nd Year Game DEV\Maya Projects 2025-2026\Maya Assessment Group work\GamesProduction_Assessment3\Group1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD6D944-3EF3-450F-8964-2F28D2C1A954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E7118C-07D8-470B-B657-36CAAA8B6D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2498" yWindow="1965" windowWidth="14400" windowHeight="8183" xr2:uid="{3CADAA71-2A7C-4007-B115-84B73D999E61}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{3CADAA71-2A7C-4007-B115-84B73D999E61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="74">
   <si>
     <t>Number</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Character 3 With Animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F </t>
+  </si>
+  <si>
+    <t>Bookshelf with books</t>
   </si>
 </sst>
 </file>
@@ -617,12 +623,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2F9C19-B13F-4412-8794-4506A44CE5A9}">
   <dimension ref="A1:G300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="103" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="103" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="10.265625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="3" width="27.796875" customWidth="1"/>
     <col min="4" max="4" width="8.86328125" customWidth="1"/>
   </cols>
@@ -1099,8 +1107,14 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
       <c r="B41" s="1" t="s">
-        <v>5</v>
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
edits and updates to the scene
</commit_message>
<xml_diff>
--- a/Group1/asset_list.xlsx
+++ b/Group1/asset_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakri\Downloads\UNIVERSITY\2nd Year Game DEV\Maya Projects 2025-2026\Maya Assessment Group work\GamesProduction_Assessment3\Group1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronni\OneDrive\Documents\GitHub\GamesProduction_Assessment3\Group1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E7118C-07D8-470B-B657-36CAAA8B6D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BE02B6-6E5A-44C0-ABE9-4502A73C72D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{3CADAA71-2A7C-4007-B115-84B73D999E61}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3CADAA71-2A7C-4007-B115-84B73D999E61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -623,19 +623,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2F9C19-B13F-4412-8794-4506A44CE5A9}">
   <dimension ref="A1:G300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="103" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="103" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.265625" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" customWidth="1"/>
-    <col min="3" max="3" width="27.796875" customWidth="1"/>
-    <col min="4" max="4" width="8.86328125" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -656,7 +656,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -670,7 +670,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -684,7 +684,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -698,7 +698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -712,7 +712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -723,7 +723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -734,7 +734,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -745,7 +745,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -756,7 +756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -776,7 +776,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -787,7 +787,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -798,7 +798,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -809,7 +809,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -820,7 +820,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -831,7 +831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -842,7 +842,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -853,7 +853,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -864,7 +864,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -875,7 +875,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -886,7 +886,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -897,7 +897,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -908,7 +908,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -919,7 +919,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -930,7 +930,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -941,7 +941,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -952,7 +952,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -963,7 +963,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -974,7 +974,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -985,7 +985,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -996,7 +996,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -1117,1297 +1117,1297 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B129" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B133" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B134" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B144" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B145" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B146" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B147" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B148" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B149" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B151" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B152" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B153" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B154" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B155" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B156" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B157" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B158" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B159" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B160" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B161" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B162" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B163" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B164" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B165" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B166" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B167" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B168" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B169" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B170" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B171" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B172" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B173" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B174" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B175" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B176" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B177" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B178" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B179" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B180" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B181" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B182" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B183" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B184" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B185" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B186" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B187" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B188" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B189" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B190" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B191" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B192" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B193" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B194" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B195" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B196" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B197" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B198" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B199" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B200" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B201" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B202" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B203" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B204" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B205" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B206" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B207" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B208" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B209" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B210" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B211" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B212" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B213" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B214" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B215" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B216" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B217" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B218" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B219" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B220" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B221" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B222" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B223" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B224" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B225" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B226" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B227" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B228" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B229" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B230" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B231" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B232" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B233" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B234" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B235" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B236" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B237" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B238" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B239" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B240" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B241" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B242" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B243" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B244" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B245" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B246" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B247" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B248" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B249" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B250" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B251" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B252" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B253" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B254" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B255" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B256" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B257" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B258" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B259" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B260" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B261" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B262" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B263" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B264" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B265" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B266" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B267" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B268" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B269" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B270" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B271" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B272" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B273" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B274" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B275" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B276" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B277" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B278" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B279" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B280" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B281" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B282" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B283" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B284" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B285" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B286" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B287" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B288" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="289" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B289" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="290" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B290" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="291" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B291" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="292" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B292" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B293" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B294" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="295" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B295" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="296" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B296" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="297" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B297" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="298" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B298" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B299" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="300" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B300" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>